<commit_message>
Added a picture for the training progress.
</commit_message>
<xml_diff>
--- a/ProbQA/Notes/Metrics/TrainingProgress/LinearPriority.xlsx
+++ b/ProbQA/Notes/Metrics/TrainingProgress/LinearPriority.xlsx
@@ -6134,11 +6134,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1838332000"/>
-        <c:axId val="-1838332544"/>
+        <c:axId val="-1742204944"/>
+        <c:axId val="-1742200592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1838332000"/>
+        <c:axId val="-1742204944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5100000"/>
@@ -6160,7 +6160,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6197,12 +6197,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1838332544"/>
+        <c:crossAx val="-1742200592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1838332544"/>
+        <c:axId val="-1742200592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -6260,7 +6260,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1838332000"/>
+        <c:crossAx val="-1742204944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7168,7 +7168,7 @@
   <dimension ref="A1:C2675"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added experiments with priority functions.
</commit_message>
<xml_diff>
--- a/ProbQA/Notes/Metrics/TrainingProgress/LinearPriority.xlsx
+++ b/ProbQA/Notes/Metrics/TrainingProgress/LinearPriority.xlsx
@@ -6134,11 +6134,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1742204944"/>
-        <c:axId val="-1742200592"/>
+        <c:axId val="-25002912"/>
+        <c:axId val="-25009440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1742204944"/>
+        <c:axId val="-25002912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5100000"/>
@@ -6197,12 +6197,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1742200592"/>
+        <c:crossAx val="-25009440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1742200592"/>
+        <c:axId val="-25009440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -6260,7 +6260,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1742204944"/>
+        <c:crossAx val="-25002912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7168,7 +7168,7 @@
   <dimension ref="A1:C2675"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="B910" sqref="B910"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>